<commit_message>
sorted out the defines for the com protocol on the stm32 and added a packet to tell if the board managed to connect to internet
</commit_message>
<xml_diff>
--- a/DOC/Packet Structure.xlsx
+++ b/DOC/Packet Structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ProiectLicenta\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B40EE8-4627-4912-BBBD-F298356F1081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A14956-B6A9-4AB8-ACE6-35DC82C462ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documantation" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
   <si>
     <t>HEAD</t>
   </si>
@@ -183,12 +183,6 @@
     <t>TIME STAMP</t>
   </si>
   <si>
-    <t>PTDB 00</t>
-  </si>
-  <si>
-    <t>ST 07</t>
-  </si>
-  <si>
     <t>0x18</t>
   </si>
   <si>
@@ -201,24 +195,6 @@
     <t>0x0B</t>
   </si>
   <si>
-    <t>YEAR 01</t>
-  </si>
-  <si>
-    <t>MONTH 02</t>
-  </si>
-  <si>
-    <t>DAY 03</t>
-  </si>
-  <si>
-    <t>HOUR 04</t>
-  </si>
-  <si>
-    <t>MINUTE 05</t>
-  </si>
-  <si>
-    <t>SECOND 06</t>
-  </si>
-  <si>
     <t>START</t>
   </si>
   <si>
@@ -247,6 +223,15 @@
   </si>
   <si>
     <t>0x03</t>
+  </si>
+  <si>
+    <t>HOUR</t>
+  </si>
+  <si>
+    <t>MINUTE</t>
+  </si>
+  <si>
+    <t>SECOND</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1446,7 +1431,235 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1457,18 +1670,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1544,24 +1748,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1571,187 +1757,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1760,18 +1787,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1788,39 +1803,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2121,7 +2103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E5:X46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C12" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
@@ -2139,26 +2121,26 @@
   <sheetData>
     <row r="5" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="5:22" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="82" t="s">
+      <c r="E6" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="76" t="s">
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="82" t="s">
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="55"/>
+      <c r="Q6" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="R6" s="83"/>
+      <c r="R6" s="60"/>
       <c r="T6" s="13" t="s">
         <v>29</v>
       </c>
@@ -2170,20 +2152,20 @@
       </c>
     </row>
     <row r="7" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="108"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="80"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="84"/>
-      <c r="R7" s="85"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="58"/>
+      <c r="Q7" s="61"/>
+      <c r="R7" s="62"/>
       <c r="T7" s="13" t="s">
         <v>30</v>
       </c>
@@ -2195,30 +2177,30 @@
       </c>
     </row>
     <row r="8" spans="5:22" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="100"/>
-      <c r="G8" s="103" t="s">
+      <c r="E8" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="76"/>
+      <c r="G8" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="104"/>
-      <c r="I8" s="117" t="s">
+      <c r="H8" s="80"/>
+      <c r="I8" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="118"/>
-      <c r="K8" s="111" t="s">
+      <c r="J8" s="94"/>
+      <c r="K8" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="112"/>
-      <c r="M8" s="112"/>
-      <c r="N8" s="112"/>
-      <c r="O8" s="112"/>
-      <c r="P8" s="113"/>
-      <c r="Q8" s="72" t="s">
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="89"/>
+      <c r="Q8" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="R8" s="73"/>
+      <c r="R8" s="50"/>
       <c r="T8" s="13" t="s">
         <v>39</v>
       </c>
@@ -2230,20 +2212,20 @@
       </c>
     </row>
     <row r="9" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="101"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="105"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="119"/>
-      <c r="J9" s="120"/>
-      <c r="K9" s="114"/>
-      <c r="L9" s="115"/>
-      <c r="M9" s="115"/>
-      <c r="N9" s="115"/>
-      <c r="O9" s="115"/>
-      <c r="P9" s="116"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="75"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="95"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="91"/>
+      <c r="N9" s="91"/>
+      <c r="O9" s="91"/>
+      <c r="P9" s="92"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="52"/>
       <c r="T9" s="13" t="s">
         <v>41</v>
       </c>
@@ -2255,34 +2237,34 @@
       </c>
     </row>
     <row r="10" spans="5:22" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="121" t="s">
+      <c r="E10" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="96"/>
-      <c r="G10" s="121" t="s">
+      <c r="F10" s="31"/>
+      <c r="G10" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="95"/>
-      <c r="I10" s="121" t="s">
+      <c r="H10" s="28"/>
+      <c r="I10" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="96"/>
-      <c r="K10" s="121" t="s">
+      <c r="J10" s="31"/>
+      <c r="K10" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="96"/>
-      <c r="M10" s="95" t="s">
+      <c r="L10" s="31"/>
+      <c r="M10" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="N10" s="95"/>
-      <c r="O10" s="121" t="s">
+      <c r="N10" s="28"/>
+      <c r="O10" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="P10" s="96"/>
-      <c r="Q10" s="95" t="s">
+      <c r="P10" s="31"/>
+      <c r="Q10" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="R10" s="96"/>
+      <c r="R10" s="31"/>
       <c r="T10" s="13" t="s">
         <v>26</v>
       </c>
@@ -2294,20 +2276,20 @@
       </c>
     </row>
     <row r="11" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="122"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="122"/>
-      <c r="H11" s="97"/>
-      <c r="I11" s="122"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="122"/>
-      <c r="L11" s="98"/>
-      <c r="M11" s="97"/>
-      <c r="N11" s="97"/>
-      <c r="O11" s="122"/>
-      <c r="P11" s="98"/>
-      <c r="Q11" s="97"/>
-      <c r="R11" s="98"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="32"/>
       <c r="T11" s="13" t="s">
         <v>31</v>
       </c>
@@ -2321,15 +2303,15 @@
     <row r="12" spans="5:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="5:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="24" t="str">
+      <c r="E15" s="63" t="str">
         <f>E6</f>
         <v>HEADER BYTES</v>
       </c>
-      <c r="F15" s="25"/>
+      <c r="F15" s="64"/>
     </row>
     <row r="16" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="86"/>
-      <c r="F16" s="27"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66"/>
     </row>
     <row r="17" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E17" s="4"/>
@@ -2337,34 +2319,34 @@
     <row r="18" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" s="3"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="87" t="str">
+      <c r="G18" s="67" t="str">
         <f>E8</f>
         <v>START</v>
       </c>
-      <c r="H18" s="88"/>
-      <c r="I18" s="53" t="s">
+      <c r="H18" s="68"/>
+      <c r="I18" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="55"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="39"/>
     </row>
     <row r="19" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E19" s="2"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="57"/>
-      <c r="O19" s="57"/>
-      <c r="P19" s="58"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="42"/>
     </row>
     <row r="20" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20" s="2"/>
@@ -2372,195 +2354,195 @@
     <row r="21" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E21" s="2"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="91" t="str">
+      <c r="G21" s="71" t="str">
         <f>G8</f>
         <v>DATA SIZE</v>
       </c>
-      <c r="H21" s="92"/>
-      <c r="I21" s="66" t="s">
+      <c r="H21" s="72"/>
+      <c r="I21" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="67"/>
-      <c r="M21" s="67"/>
-      <c r="N21" s="67"/>
-      <c r="O21" s="67"/>
-      <c r="P21" s="68"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="45"/>
     </row>
     <row r="22" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G22" s="93"/>
-      <c r="H22" s="94"/>
-      <c r="I22" s="69"/>
-      <c r="J22" s="70"/>
-      <c r="K22" s="70"/>
-      <c r="L22" s="70"/>
-      <c r="M22" s="70"/>
-      <c r="N22" s="70"/>
-      <c r="O22" s="70"/>
-      <c r="P22" s="71"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="48"/>
     </row>
     <row r="23" spans="5:24" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="5:24" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="62" t="str">
+      <c r="E25" s="33" t="str">
         <f>I6</f>
         <v>DATA BYTES</v>
       </c>
-      <c r="F25" s="63"/>
+      <c r="F25" s="34"/>
     </row>
     <row r="26" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="64"/>
-      <c r="F26" s="65"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E28" s="3"/>
-      <c r="G28" s="49" t="str">
+      <c r="G28" s="122" t="str">
         <f>I8</f>
         <v>PACKET TYPE</v>
       </c>
-      <c r="H28" s="50"/>
-      <c r="I28" s="53" t="s">
+      <c r="H28" s="123"/>
+      <c r="I28" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="J28" s="54"/>
-      <c r="K28" s="54"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="59" t="s">
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="N28" s="60"/>
-      <c r="O28" s="60"/>
-      <c r="P28" s="61"/>
-      <c r="R28" s="135"/>
-      <c r="S28" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="T28" s="20"/>
-      <c r="U28" s="20"/>
-      <c r="V28" s="20"/>
-      <c r="W28" s="20"/>
-      <c r="X28" s="20"/>
+      <c r="N28" s="127"/>
+      <c r="O28" s="127"/>
+      <c r="P28" s="128"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="129" t="s">
+        <v>56</v>
+      </c>
+      <c r="T28" s="129"/>
+      <c r="U28" s="129"/>
+      <c r="V28" s="129"/>
+      <c r="W28" s="129"/>
+      <c r="X28" s="129"/>
     </row>
     <row r="29" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E29" s="2"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="58"/>
-      <c r="M29" s="59" t="s">
+      <c r="G29" s="124"/>
+      <c r="H29" s="125"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="N29" s="60"/>
-      <c r="O29" s="60"/>
-      <c r="P29" s="61"/>
-      <c r="R29" s="135"/>
-      <c r="S29" s="20"/>
-      <c r="T29" s="20"/>
-      <c r="U29" s="20"/>
-      <c r="V29" s="20"/>
-      <c r="W29" s="20"/>
-      <c r="X29" s="20"/>
+      <c r="N29" s="127"/>
+      <c r="O29" s="127"/>
+      <c r="P29" s="128"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="129"/>
+      <c r="T29" s="129"/>
+      <c r="U29" s="129"/>
+      <c r="V29" s="129"/>
+      <c r="W29" s="129"/>
+      <c r="X29" s="129"/>
     </row>
     <row r="30" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E30" s="2"/>
-      <c r="R30" s="135"/>
-      <c r="S30" s="20"/>
-      <c r="T30" s="20"/>
-      <c r="U30" s="20"/>
-      <c r="V30" s="20"/>
-      <c r="W30" s="20"/>
-      <c r="X30" s="20"/>
+      <c r="R30" s="20"/>
+      <c r="S30" s="129"/>
+      <c r="T30" s="129"/>
+      <c r="U30" s="129"/>
+      <c r="V30" s="129"/>
+      <c r="W30" s="129"/>
+      <c r="X30" s="129"/>
     </row>
     <row r="31" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E31" s="2"/>
-      <c r="G31" s="38" t="s">
+      <c r="G31" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="39"/>
-      <c r="I31" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="44"/>
-      <c r="P31" s="45"/>
-      <c r="R31" s="135"/>
-      <c r="S31" s="20"/>
-      <c r="T31" s="20"/>
-      <c r="U31" s="20"/>
-      <c r="V31" s="20"/>
-      <c r="W31" s="20"/>
-      <c r="X31" s="20"/>
+      <c r="H31" s="112"/>
+      <c r="I31" s="116" t="s">
+        <v>53</v>
+      </c>
+      <c r="J31" s="117"/>
+      <c r="K31" s="117"/>
+      <c r="L31" s="117"/>
+      <c r="M31" s="117"/>
+      <c r="N31" s="117"/>
+      <c r="O31" s="117"/>
+      <c r="P31" s="118"/>
+      <c r="R31" s="20"/>
+      <c r="S31" s="129"/>
+      <c r="T31" s="129"/>
+      <c r="U31" s="129"/>
+      <c r="V31" s="129"/>
+      <c r="W31" s="129"/>
+      <c r="X31" s="129"/>
     </row>
     <row r="32" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F32" s="8"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
-      <c r="P32" s="48"/>
-      <c r="R32" s="135"/>
-      <c r="S32" s="20"/>
-      <c r="T32" s="20"/>
-      <c r="U32" s="20"/>
-      <c r="V32" s="20"/>
-      <c r="W32" s="20"/>
-      <c r="X32" s="20"/>
+      <c r="G32" s="113"/>
+      <c r="H32" s="114"/>
+      <c r="I32" s="119"/>
+      <c r="J32" s="120"/>
+      <c r="K32" s="120"/>
+      <c r="L32" s="120"/>
+      <c r="M32" s="120"/>
+      <c r="N32" s="120"/>
+      <c r="O32" s="120"/>
+      <c r="P32" s="121"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="129"/>
+      <c r="T32" s="129"/>
+      <c r="U32" s="129"/>
+      <c r="V32" s="129"/>
+      <c r="W32" s="129"/>
+      <c r="X32" s="129"/>
     </row>
     <row r="33" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G33" s="9"/>
-      <c r="R33" s="135"/>
-      <c r="S33" s="20"/>
-      <c r="T33" s="20"/>
-      <c r="U33" s="20"/>
-      <c r="V33" s="20"/>
-      <c r="W33" s="20"/>
-      <c r="X33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="129"/>
+      <c r="T33" s="129"/>
+      <c r="U33" s="129"/>
+      <c r="V33" s="129"/>
+      <c r="W33" s="129"/>
+      <c r="X33" s="129"/>
     </row>
     <row r="34" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="42" t="s">
+      <c r="G34" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="42"/>
-      <c r="I34" s="136" t="s">
+      <c r="H34" s="115"/>
+      <c r="I34" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="J34" s="137"/>
-      <c r="K34" s="137"/>
-      <c r="L34" s="137"/>
-      <c r="M34" s="137"/>
-      <c r="N34" s="137"/>
-      <c r="O34" s="140"/>
-      <c r="P34" s="141"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="26"/>
       <c r="Q34" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="R34" s="135"/>
-      <c r="S34" s="20"/>
-      <c r="T34" s="20"/>
-      <c r="U34" s="20"/>
-      <c r="V34" s="20"/>
-      <c r="W34" s="20"/>
-      <c r="X34" s="20"/>
+      <c r="R34" s="20"/>
+      <c r="S34" s="129"/>
+      <c r="T34" s="129"/>
+      <c r="U34" s="129"/>
+      <c r="V34" s="129"/>
+      <c r="W34" s="129"/>
+      <c r="X34" s="129"/>
     </row>
     <row r="35" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
+      <c r="G35" s="115"/>
+      <c r="H35" s="115"/>
       <c r="I35" s="10" t="s">
         <v>16</v>
       </c>
@@ -2576,158 +2558,159 @@
       <c r="M35" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="138" t="s">
+      <c r="N35" s="21" t="s">
         <v>21</v>
       </c>
       <c r="O35" s="10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="P35" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q35" s="139" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q35" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="R35" s="135"/>
-      <c r="S35" s="20"/>
-      <c r="T35" s="20"/>
-      <c r="U35" s="20"/>
-      <c r="V35" s="20"/>
-      <c r="W35" s="20"/>
-      <c r="X35" s="20"/>
+      <c r="R35" s="20"/>
+      <c r="S35" s="129"/>
+      <c r="T35" s="129"/>
+      <c r="U35" s="129"/>
+      <c r="V35" s="129"/>
+      <c r="W35" s="129"/>
+      <c r="X35" s="129"/>
     </row>
     <row r="36" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G36" s="11"/>
-      <c r="R36" s="135"/>
-      <c r="S36" s="20"/>
-      <c r="T36" s="20"/>
-      <c r="U36" s="20"/>
-      <c r="V36" s="20"/>
-      <c r="W36" s="20"/>
-      <c r="X36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="129"/>
+      <c r="T36" s="129"/>
+      <c r="U36" s="129"/>
+      <c r="V36" s="129"/>
+      <c r="W36" s="129"/>
+      <c r="X36" s="129"/>
     </row>
     <row r="37" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="G37" s="22" t="s">
+      <c r="G37" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22" t="s">
+      <c r="H37" s="98"/>
+      <c r="I37" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
-      <c r="R37" s="135"/>
-      <c r="S37" s="20"/>
-      <c r="T37" s="20"/>
-      <c r="U37" s="20"/>
-      <c r="V37" s="20"/>
-      <c r="W37" s="20"/>
-      <c r="X37" s="20"/>
+      <c r="J37" s="98"/>
+      <c r="K37" s="98"/>
+      <c r="L37" s="98"/>
+      <c r="M37" s="98"/>
+      <c r="N37" s="98"/>
+      <c r="O37" s="98"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="129"/>
+      <c r="T37" s="129"/>
+      <c r="U37" s="129"/>
+      <c r="V37" s="129"/>
+      <c r="W37" s="129"/>
+      <c r="X37" s="129"/>
     </row>
     <row r="38" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="23"/>
-      <c r="R38" s="135"/>
-      <c r="S38" s="20"/>
-      <c r="T38" s="20"/>
-      <c r="U38" s="20"/>
-      <c r="V38" s="20"/>
-      <c r="W38" s="20"/>
-      <c r="X38" s="20"/>
+      <c r="G38" s="99"/>
+      <c r="H38" s="99"/>
+      <c r="I38" s="99"/>
+      <c r="J38" s="99"/>
+      <c r="K38" s="99"/>
+      <c r="L38" s="99"/>
+      <c r="M38" s="99"/>
+      <c r="N38" s="99"/>
+      <c r="O38" s="99"/>
+      <c r="R38" s="20"/>
+      <c r="S38" s="129"/>
+      <c r="T38" s="129"/>
+      <c r="U38" s="129"/>
+      <c r="V38" s="129"/>
+      <c r="W38" s="129"/>
+      <c r="X38" s="129"/>
     </row>
     <row r="40" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="5:24" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E41" s="24" t="str">
+      <c r="E41" s="63" t="str">
         <f>Q6</f>
         <v>END BYTE</v>
       </c>
-      <c r="F41" s="25"/>
+      <c r="F41" s="64"/>
     </row>
     <row r="42" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E42" s="26"/>
-      <c r="F42" s="27"/>
+      <c r="E42" s="100"/>
+      <c r="F42" s="66"/>
     </row>
     <row r="43" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E43" s="4"/>
-      <c r="R43" s="21" t="s">
+      <c r="R43" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="S43" s="21"/>
-      <c r="T43" s="21"/>
-      <c r="U43" s="21"/>
-      <c r="V43" s="21"/>
-      <c r="W43" s="21"/>
+      <c r="S43" s="97"/>
+      <c r="T43" s="97"/>
+      <c r="U43" s="97"/>
+      <c r="V43" s="97"/>
+      <c r="W43" s="97"/>
     </row>
     <row r="44" spans="5:24" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E44" s="3"/>
-      <c r="G44" s="28" t="str">
+      <c r="G44" s="101" t="str">
         <f>Q8</f>
         <v>CHECK SUM</v>
       </c>
-      <c r="H44" s="29"/>
-      <c r="I44" s="32" t="s">
+      <c r="H44" s="102"/>
+      <c r="I44" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="J44" s="33"/>
-      <c r="K44" s="33"/>
-      <c r="L44" s="33"/>
-      <c r="M44" s="33"/>
-      <c r="N44" s="33"/>
-      <c r="O44" s="33"/>
-      <c r="P44" s="34"/>
-      <c r="R44" s="21"/>
-      <c r="S44" s="21"/>
-      <c r="T44" s="21"/>
-      <c r="U44" s="21"/>
-      <c r="V44" s="21"/>
-      <c r="W44" s="21"/>
+      <c r="J44" s="106"/>
+      <c r="K44" s="106"/>
+      <c r="L44" s="106"/>
+      <c r="M44" s="106"/>
+      <c r="N44" s="106"/>
+      <c r="O44" s="106"/>
+      <c r="P44" s="107"/>
+      <c r="R44" s="97"/>
+      <c r="S44" s="97"/>
+      <c r="T44" s="97"/>
+      <c r="U44" s="97"/>
+      <c r="V44" s="97"/>
+      <c r="W44" s="97"/>
     </row>
     <row r="45" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F45" s="12"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="36"/>
-      <c r="L45" s="36"/>
-      <c r="M45" s="36"/>
-      <c r="N45" s="36"/>
-      <c r="O45" s="36"/>
-      <c r="P45" s="37"/>
-      <c r="R45" s="21"/>
-      <c r="S45" s="21"/>
-      <c r="T45" s="21"/>
-      <c r="U45" s="21"/>
-      <c r="V45" s="21"/>
-      <c r="W45" s="21"/>
+      <c r="G45" s="103"/>
+      <c r="H45" s="104"/>
+      <c r="I45" s="108"/>
+      <c r="J45" s="109"/>
+      <c r="K45" s="109"/>
+      <c r="L45" s="109"/>
+      <c r="M45" s="109"/>
+      <c r="N45" s="109"/>
+      <c r="O45" s="109"/>
+      <c r="P45" s="110"/>
+      <c r="R45" s="97"/>
+      <c r="S45" s="97"/>
+      <c r="T45" s="97"/>
+      <c r="U45" s="97"/>
+      <c r="V45" s="97"/>
+      <c r="W45" s="97"/>
     </row>
     <row r="46" spans="5:24" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="R46" s="21"/>
-      <c r="S46" s="21"/>
-      <c r="T46" s="21"/>
-      <c r="U46" s="21"/>
-      <c r="V46" s="21"/>
-      <c r="W46" s="21"/>
+      <c r="R46" s="97"/>
+      <c r="S46" s="97"/>
+      <c r="T46" s="97"/>
+      <c r="U46" s="97"/>
+      <c r="V46" s="97"/>
+      <c r="W46" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="I34:P34"/>
-    <mergeCell ref="G10:H11"/>
-    <mergeCell ref="I10:J11"/>
-    <mergeCell ref="K10:L11"/>
-    <mergeCell ref="M10:N11"/>
-    <mergeCell ref="O10:P11"/>
+    <mergeCell ref="R43:W46"/>
+    <mergeCell ref="G37:H38"/>
+    <mergeCell ref="I37:O38"/>
+    <mergeCell ref="E41:F42"/>
+    <mergeCell ref="G44:H45"/>
+    <mergeCell ref="I44:P45"/>
+    <mergeCell ref="S28:X38"/>
     <mergeCell ref="E25:F26"/>
     <mergeCell ref="I18:P19"/>
     <mergeCell ref="I21:P22"/>
@@ -2744,12 +2727,12 @@
     <mergeCell ref="K8:P9"/>
     <mergeCell ref="I8:J9"/>
     <mergeCell ref="E10:F11"/>
-    <mergeCell ref="R43:W46"/>
-    <mergeCell ref="G37:H38"/>
-    <mergeCell ref="I37:O38"/>
-    <mergeCell ref="E41:F42"/>
-    <mergeCell ref="G44:H45"/>
-    <mergeCell ref="I44:P45"/>
+    <mergeCell ref="I34:P34"/>
+    <mergeCell ref="G10:H11"/>
+    <mergeCell ref="I10:J11"/>
+    <mergeCell ref="K10:L11"/>
+    <mergeCell ref="M10:N11"/>
+    <mergeCell ref="O10:P11"/>
     <mergeCell ref="G31:H32"/>
     <mergeCell ref="G34:H35"/>
     <mergeCell ref="I31:P32"/>
@@ -2757,7 +2740,6 @@
     <mergeCell ref="I28:L29"/>
     <mergeCell ref="M28:P28"/>
     <mergeCell ref="M29:P29"/>
-    <mergeCell ref="S28:X38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2768,8 +2750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F8F41-6AB8-4FE5-9A10-D5070C0839ED}">
   <dimension ref="B1:AJ32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="AF25" sqref="AF25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AI19" sqref="AI19:AJ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2784,130 +2766,130 @@
   <sheetData>
     <row r="1" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:36" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="125" t="s">
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="127"/>
-      <c r="N2" s="82" t="s">
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="132"/>
+      <c r="N2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="83"/>
+      <c r="O2" s="60"/>
     </row>
     <row r="3" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="108"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="85"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="62"/>
     </row>
     <row r="4" spans="2:36" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="103" t="s">
+      <c r="C4" s="76"/>
+      <c r="D4" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="104"/>
-      <c r="F4" s="117" t="s">
+      <c r="E4" s="80"/>
+      <c r="F4" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="118"/>
-      <c r="H4" s="111" t="s">
+      <c r="G4" s="94"/>
+      <c r="H4" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="112"/>
-      <c r="M4" s="113"/>
-      <c r="N4" s="72" t="s">
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="73"/>
+      <c r="O4" s="50"/>
     </row>
     <row r="5" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="101"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="115"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="116"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="75"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="52"/>
     </row>
     <row r="6" spans="2:36" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="121" t="s">
+      <c r="C6" s="31"/>
+      <c r="D6" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="95"/>
-      <c r="F6" s="121" t="s">
+      <c r="E6" s="28"/>
+      <c r="F6" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="121" t="s">
+      <c r="G6" s="31"/>
+      <c r="H6" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="96"/>
-      <c r="J6" s="95" t="s">
+      <c r="I6" s="31"/>
+      <c r="J6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="95"/>
-      <c r="L6" s="121" t="s">
+      <c r="K6" s="28"/>
+      <c r="L6" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="96"/>
-      <c r="N6" s="95" t="s">
+      <c r="M6" s="31"/>
+      <c r="N6" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="96"/>
+      <c r="O6" s="31"/>
     </row>
     <row r="7" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="122"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="97"/>
-      <c r="F7" s="122"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="122"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="97"/>
-      <c r="K7" s="97"/>
-      <c r="L7" s="122"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="97"/>
-      <c r="O7" s="98"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="32"/>
     </row>
     <row r="8" spans="2:36" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:36" x14ac:dyDescent="0.25">
@@ -2915,403 +2897,403 @@
         <v>44</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:36" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="107"/>
-      <c r="D15" s="107"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="125" t="s">
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="126"/>
-      <c r="H15" s="82" t="s">
+      <c r="G15" s="131"/>
+      <c r="H15" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="83"/>
+      <c r="I15" s="60"/>
       <c r="J15" s="16"/>
-      <c r="K15" s="82" t="s">
+      <c r="K15" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="L15" s="107"/>
-      <c r="M15" s="107"/>
-      <c r="N15" s="83"/>
-      <c r="O15" s="76" t="s">
+      <c r="L15" s="83"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="P15" s="77"/>
-      <c r="Q15" s="77"/>
-      <c r="R15" s="77"/>
-      <c r="S15" s="77"/>
-      <c r="T15" s="77"/>
-      <c r="U15" s="77"/>
-      <c r="V15" s="77"/>
-      <c r="W15" s="77"/>
-      <c r="X15" s="77"/>
-      <c r="Y15" s="77"/>
-      <c r="Z15" s="77"/>
-      <c r="AA15" s="77"/>
-      <c r="AB15" s="77"/>
-      <c r="AC15" s="77"/>
-      <c r="AD15" s="77"/>
-      <c r="AE15" s="77"/>
-      <c r="AF15" s="77"/>
-      <c r="AG15" s="77"/>
-      <c r="AH15" s="78"/>
-      <c r="AI15" s="82" t="s">
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="54"/>
+      <c r="T15" s="54"/>
+      <c r="U15" s="54"/>
+      <c r="V15" s="54"/>
+      <c r="W15" s="54"/>
+      <c r="X15" s="54"/>
+      <c r="Y15" s="54"/>
+      <c r="Z15" s="54"/>
+      <c r="AA15" s="54"/>
+      <c r="AB15" s="54"/>
+      <c r="AC15" s="54"/>
+      <c r="AD15" s="54"/>
+      <c r="AE15" s="54"/>
+      <c r="AF15" s="54"/>
+      <c r="AG15" s="54"/>
+      <c r="AH15" s="55"/>
+      <c r="AI15" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="AJ15" s="83"/>
+      <c r="AJ15" s="60"/>
     </row>
     <row r="16" spans="2:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="108"/>
-      <c r="C16" s="109"/>
-      <c r="D16" s="109"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="129"/>
-      <c r="G16" s="130"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="85"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="139"/>
+      <c r="G16" s="140"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="62"/>
       <c r="J16" s="16"/>
-      <c r="K16" s="108"/>
-      <c r="L16" s="109"/>
-      <c r="M16" s="109"/>
-      <c r="N16" s="110"/>
-      <c r="O16" s="79"/>
-      <c r="P16" s="142"/>
-      <c r="Q16" s="142"/>
-      <c r="R16" s="142"/>
-      <c r="S16" s="142"/>
-      <c r="T16" s="142"/>
-      <c r="U16" s="142"/>
-      <c r="V16" s="142"/>
-      <c r="W16" s="142"/>
-      <c r="X16" s="142"/>
-      <c r="Y16" s="142"/>
-      <c r="Z16" s="142"/>
-      <c r="AA16" s="142"/>
-      <c r="AB16" s="142"/>
-      <c r="AC16" s="142"/>
-      <c r="AD16" s="142"/>
-      <c r="AE16" s="142"/>
-      <c r="AF16" s="142"/>
-      <c r="AG16" s="142"/>
-      <c r="AH16" s="81"/>
-      <c r="AI16" s="84"/>
-      <c r="AJ16" s="85"/>
+      <c r="K16" s="84"/>
+      <c r="L16" s="85"/>
+      <c r="M16" s="85"/>
+      <c r="N16" s="86"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="57"/>
+      <c r="S16" s="57"/>
+      <c r="T16" s="57"/>
+      <c r="U16" s="57"/>
+      <c r="V16" s="57"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
+      <c r="Y16" s="57"/>
+      <c r="Z16" s="57"/>
+      <c r="AA16" s="57"/>
+      <c r="AB16" s="57"/>
+      <c r="AC16" s="57"/>
+      <c r="AD16" s="57"/>
+      <c r="AE16" s="57"/>
+      <c r="AF16" s="57"/>
+      <c r="AG16" s="57"/>
+      <c r="AH16" s="58"/>
+      <c r="AI16" s="61"/>
+      <c r="AJ16" s="62"/>
     </row>
     <row r="17" spans="2:36" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="100"/>
-      <c r="D17" s="103" t="s">
+      <c r="C17" s="76"/>
+      <c r="D17" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="104"/>
-      <c r="F17" s="117" t="s">
+      <c r="E17" s="80"/>
+      <c r="F17" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="118"/>
-      <c r="H17" s="131" t="s">
+      <c r="G17" s="94"/>
+      <c r="H17" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="132"/>
+      <c r="I17" s="142"/>
       <c r="J17" s="16"/>
-      <c r="K17" s="99" t="s">
+      <c r="K17" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="L17" s="100"/>
-      <c r="M17" s="103" t="s">
+      <c r="L17" s="76"/>
+      <c r="M17" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="N17" s="104"/>
-      <c r="O17" s="117" t="s">
+      <c r="N17" s="80"/>
+      <c r="O17" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="P17" s="118"/>
-      <c r="Q17" s="111" t="s">
+      <c r="P17" s="94"/>
+      <c r="Q17" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="112"/>
-      <c r="S17" s="112"/>
-      <c r="T17" s="112"/>
-      <c r="U17" s="112"/>
-      <c r="V17" s="112"/>
-      <c r="W17" s="112"/>
-      <c r="X17" s="112"/>
-      <c r="Y17" s="112"/>
-      <c r="Z17" s="112"/>
-      <c r="AA17" s="112"/>
-      <c r="AB17" s="112"/>
-      <c r="AC17" s="112"/>
-      <c r="AD17" s="112"/>
-      <c r="AE17" s="112"/>
-      <c r="AF17" s="128"/>
-      <c r="AG17" s="111" t="s">
+      <c r="R17" s="88"/>
+      <c r="S17" s="88"/>
+      <c r="T17" s="88"/>
+      <c r="U17" s="88"/>
+      <c r="V17" s="88"/>
+      <c r="W17" s="88"/>
+      <c r="X17" s="88"/>
+      <c r="Y17" s="88"/>
+      <c r="Z17" s="88"/>
+      <c r="AA17" s="88"/>
+      <c r="AB17" s="88"/>
+      <c r="AC17" s="88"/>
+      <c r="AD17" s="88"/>
+      <c r="AE17" s="88"/>
+      <c r="AF17" s="133"/>
+      <c r="AG17" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="AH17" s="113"/>
-      <c r="AI17" s="72" t="s">
+      <c r="AH17" s="89"/>
+      <c r="AI17" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="AJ17" s="73"/>
+      <c r="AJ17" s="50"/>
     </row>
     <row r="18" spans="2:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="101"/>
-      <c r="C18" s="102"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="119"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="133"/>
-      <c r="I18" s="134"/>
+      <c r="B18" s="77"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="143"/>
+      <c r="I18" s="144"/>
       <c r="J18" s="16"/>
-      <c r="K18" s="101"/>
-      <c r="L18" s="102"/>
-      <c r="M18" s="105"/>
-      <c r="N18" s="106"/>
-      <c r="O18" s="119"/>
-      <c r="P18" s="120"/>
-      <c r="Q18" s="143"/>
-      <c r="R18" s="144"/>
-      <c r="S18" s="144"/>
-      <c r="T18" s="144"/>
-      <c r="U18" s="144"/>
-      <c r="V18" s="144"/>
-      <c r="W18" s="144"/>
-      <c r="X18" s="144"/>
-      <c r="Y18" s="144"/>
-      <c r="Z18" s="144"/>
-      <c r="AA18" s="144"/>
-      <c r="AB18" s="144"/>
-      <c r="AC18" s="144"/>
-      <c r="AD18" s="144"/>
-      <c r="AE18" s="144"/>
-      <c r="AF18" s="145"/>
-      <c r="AG18" s="114"/>
-      <c r="AH18" s="116"/>
-      <c r="AI18" s="74"/>
-      <c r="AJ18" s="75"/>
+      <c r="K18" s="77"/>
+      <c r="L18" s="78"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="82"/>
+      <c r="O18" s="95"/>
+      <c r="P18" s="96"/>
+      <c r="Q18" s="134"/>
+      <c r="R18" s="135"/>
+      <c r="S18" s="135"/>
+      <c r="T18" s="135"/>
+      <c r="U18" s="135"/>
+      <c r="V18" s="135"/>
+      <c r="W18" s="135"/>
+      <c r="X18" s="135"/>
+      <c r="Y18" s="135"/>
+      <c r="Z18" s="135"/>
+      <c r="AA18" s="135"/>
+      <c r="AB18" s="135"/>
+      <c r="AC18" s="135"/>
+      <c r="AD18" s="135"/>
+      <c r="AE18" s="135"/>
+      <c r="AF18" s="136"/>
+      <c r="AG18" s="90"/>
+      <c r="AH18" s="92"/>
+      <c r="AI18" s="51"/>
+      <c r="AJ18" s="52"/>
     </row>
     <row r="19" spans="2:36" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="96"/>
-      <c r="D19" s="121" t="s">
+      <c r="C19" s="31"/>
+      <c r="D19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="95"/>
-      <c r="F19" s="121" t="s">
+      <c r="E19" s="28"/>
+      <c r="F19" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="96"/>
-      <c r="H19" s="121" t="s">
+      <c r="G19" s="31"/>
+      <c r="H19" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="I19" s="96"/>
+      <c r="I19" s="31"/>
       <c r="J19" s="16"/>
-      <c r="K19" s="121" t="s">
+      <c r="K19" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="L19" s="96"/>
-      <c r="M19" s="121" t="s">
+      <c r="L19" s="31"/>
+      <c r="M19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="N19" s="95"/>
-      <c r="O19" s="121" t="s">
+      <c r="N19" s="28"/>
+      <c r="O19" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="R19" s="31"/>
+      <c r="S19" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="T19" s="28"/>
+      <c r="U19" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="V19" s="31"/>
+      <c r="W19" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="X19" s="31"/>
+      <c r="Y19" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB19" s="31"/>
+      <c r="AC19" s="145" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD19" s="145"/>
+      <c r="AE19" s="145" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF19" s="145"/>
+      <c r="AG19" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH19" s="31"/>
+      <c r="AI19" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ19" s="31"/>
+    </row>
+    <row r="20" spans="2:36" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="29"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="29"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="30"/>
+      <c r="Z20" s="30"/>
+      <c r="AA20" s="29"/>
+      <c r="AB20" s="32"/>
+      <c r="AC20" s="145"/>
+      <c r="AD20" s="145"/>
+      <c r="AE20" s="145"/>
+      <c r="AF20" s="145"/>
+      <c r="AG20" s="29"/>
+      <c r="AH20" s="32"/>
+      <c r="AI20" s="30"/>
+      <c r="AJ20" s="32"/>
+    </row>
+    <row r="21" spans="2:36" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="31"/>
+      <c r="D21" s="137" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="137"/>
+      <c r="F21" s="137" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="137"/>
+      <c r="H21" s="137" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="137"/>
+      <c r="K21" s="137" t="s">
+        <v>32</v>
+      </c>
+      <c r="L21" s="137"/>
+      <c r="M21" s="137" t="s">
+        <v>58</v>
+      </c>
+      <c r="N21" s="137"/>
+      <c r="O21" s="137" t="s">
+        <v>15</v>
+      </c>
+      <c r="P21" s="137"/>
+      <c r="Q21" s="137" t="s">
         <v>48</v>
       </c>
-      <c r="P19" s="96"/>
-      <c r="Q19" s="121" t="s">
-        <v>54</v>
-      </c>
-      <c r="R19" s="96"/>
-      <c r="S19" s="95" t="s">
-        <v>55</v>
-      </c>
-      <c r="T19" s="95"/>
-      <c r="U19" s="121" t="s">
-        <v>56</v>
-      </c>
-      <c r="V19" s="96"/>
-      <c r="W19" s="121" t="s">
-        <v>57</v>
-      </c>
-      <c r="X19" s="96"/>
-      <c r="Y19" s="95" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z19" s="95"/>
-      <c r="AA19" s="121" t="s">
+      <c r="R21" s="137"/>
+      <c r="S21" s="137" t="s">
+        <v>49</v>
+      </c>
+      <c r="T21" s="137"/>
+      <c r="U21" s="137" t="s">
+        <v>50</v>
+      </c>
+      <c r="V21" s="137"/>
+      <c r="W21" s="137" t="s">
         <v>59</v>
       </c>
-      <c r="AB19" s="96"/>
-      <c r="AC19" s="146" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD19" s="146"/>
-      <c r="AE19" s="146" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF19" s="146"/>
-      <c r="AG19" s="121" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH19" s="96"/>
-      <c r="AI19" s="95" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ19" s="96"/>
-    </row>
-    <row r="20" spans="2:36" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="122"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="122"/>
-      <c r="E20" s="97"/>
-      <c r="F20" s="122"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="122"/>
-      <c r="I20" s="98"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="122"/>
-      <c r="L20" s="98"/>
-      <c r="M20" s="122"/>
-      <c r="N20" s="97"/>
-      <c r="O20" s="122"/>
-      <c r="P20" s="98"/>
-      <c r="Q20" s="122"/>
-      <c r="R20" s="98"/>
-      <c r="S20" s="97"/>
-      <c r="T20" s="97"/>
-      <c r="U20" s="122"/>
-      <c r="V20" s="98"/>
-      <c r="W20" s="122"/>
-      <c r="X20" s="98"/>
-      <c r="Y20" s="97"/>
-      <c r="Z20" s="97"/>
-      <c r="AA20" s="122"/>
-      <c r="AB20" s="98"/>
-      <c r="AC20" s="146"/>
-      <c r="AD20" s="146"/>
-      <c r="AE20" s="146"/>
-      <c r="AF20" s="146"/>
-      <c r="AG20" s="122"/>
-      <c r="AH20" s="98"/>
-      <c r="AI20" s="97"/>
-      <c r="AJ20" s="98"/>
-    </row>
-    <row r="21" spans="2:36" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="121" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="96"/>
-      <c r="D21" s="123" t="s">
+      <c r="X21" s="137"/>
+      <c r="Y21" s="137" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z21" s="137"/>
+      <c r="AA21" s="137" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB21" s="137"/>
+      <c r="AC21" s="145" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD21" s="145"/>
+      <c r="AE21" s="145" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF21" s="145"/>
+      <c r="AG21" s="137" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="123"/>
-      <c r="F21" s="123" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="123"/>
-      <c r="H21" s="123" t="s">
+      <c r="AH21" s="137"/>
+      <c r="AI21" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="I21" s="123"/>
-      <c r="K21" s="123" t="s">
-        <v>32</v>
-      </c>
-      <c r="L21" s="123"/>
-      <c r="M21" s="123" t="s">
-        <v>66</v>
-      </c>
-      <c r="N21" s="123"/>
-      <c r="O21" s="123" t="s">
-        <v>15</v>
-      </c>
-      <c r="P21" s="123"/>
-      <c r="Q21" s="123" t="s">
-        <v>50</v>
-      </c>
-      <c r="R21" s="123"/>
-      <c r="S21" s="123" t="s">
-        <v>51</v>
-      </c>
-      <c r="T21" s="123"/>
-      <c r="U21" s="123" t="s">
-        <v>52</v>
-      </c>
-      <c r="V21" s="123"/>
-      <c r="W21" s="123" t="s">
-        <v>67</v>
-      </c>
-      <c r="X21" s="123"/>
-      <c r="Y21" s="123" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z21" s="123"/>
-      <c r="AA21" s="123" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB21" s="123"/>
-      <c r="AC21" s="146" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD21" s="146"/>
-      <c r="AE21" s="146" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF21" s="146"/>
-      <c r="AG21" s="123" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH21" s="123"/>
-      <c r="AI21" s="123" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ21" s="123"/>
+      <c r="AJ21" s="137"/>
     </row>
     <row r="22" spans="2:36" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="122"/>
-      <c r="C22" s="98"/>
-      <c r="D22" s="124"/>
-      <c r="E22" s="124"/>
-      <c r="F22" s="124"/>
-      <c r="G22" s="124"/>
-      <c r="H22" s="124"/>
-      <c r="I22" s="124"/>
-      <c r="K22" s="124"/>
-      <c r="L22" s="124"/>
-      <c r="M22" s="124"/>
-      <c r="N22" s="124"/>
-      <c r="O22" s="124"/>
-      <c r="P22" s="124"/>
-      <c r="Q22" s="124"/>
-      <c r="R22" s="124"/>
-      <c r="S22" s="124"/>
-      <c r="T22" s="124"/>
-      <c r="U22" s="124"/>
-      <c r="V22" s="124"/>
-      <c r="W22" s="124"/>
-      <c r="X22" s="124"/>
-      <c r="Y22" s="124"/>
-      <c r="Z22" s="124"/>
-      <c r="AA22" s="124"/>
-      <c r="AB22" s="124"/>
-      <c r="AC22" s="146"/>
-      <c r="AD22" s="146"/>
-      <c r="AE22" s="146"/>
-      <c r="AF22" s="146"/>
-      <c r="AG22" s="124"/>
-      <c r="AH22" s="124"/>
-      <c r="AI22" s="124"/>
-      <c r="AJ22" s="124"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="138"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="138"/>
+      <c r="G22" s="138"/>
+      <c r="H22" s="138"/>
+      <c r="I22" s="138"/>
+      <c r="K22" s="138"/>
+      <c r="L22" s="138"/>
+      <c r="M22" s="138"/>
+      <c r="N22" s="138"/>
+      <c r="O22" s="138"/>
+      <c r="P22" s="138"/>
+      <c r="Q22" s="138"/>
+      <c r="R22" s="138"/>
+      <c r="S22" s="138"/>
+      <c r="T22" s="138"/>
+      <c r="U22" s="138"/>
+      <c r="V22" s="138"/>
+      <c r="W22" s="138"/>
+      <c r="X22" s="138"/>
+      <c r="Y22" s="138"/>
+      <c r="Z22" s="138"/>
+      <c r="AA22" s="138"/>
+      <c r="AB22" s="138"/>
+      <c r="AC22" s="145"/>
+      <c r="AD22" s="145"/>
+      <c r="AE22" s="145"/>
+      <c r="AF22" s="145"/>
+      <c r="AG22" s="138"/>
+      <c r="AH22" s="138"/>
+      <c r="AI22" s="138"/>
+      <c r="AJ22" s="138"/>
     </row>
     <row r="23" spans="2:36" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:36" x14ac:dyDescent="0.25">
@@ -3336,38 +3318,23 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="F2:M3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:E5"/>
-    <mergeCell ref="F4:G5"/>
-    <mergeCell ref="H4:M5"/>
-    <mergeCell ref="N4:O5"/>
-    <mergeCell ref="N6:O7"/>
-    <mergeCell ref="B15:E16"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="D17:E18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="H6:I7"/>
-    <mergeCell ref="J6:K7"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="O15:AH16"/>
-    <mergeCell ref="Q17:AF18"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="D21:E22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="H15:I16"/>
-    <mergeCell ref="H17:I18"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="D19:E20"/>
-    <mergeCell ref="F19:G20"/>
-    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="AI19:AJ20"/>
+    <mergeCell ref="AE21:AF22"/>
+    <mergeCell ref="Y21:Z22"/>
+    <mergeCell ref="AA21:AB22"/>
+    <mergeCell ref="AG21:AH22"/>
+    <mergeCell ref="AI21:AJ22"/>
+    <mergeCell ref="O19:P20"/>
+    <mergeCell ref="Q19:R20"/>
+    <mergeCell ref="S19:T20"/>
+    <mergeCell ref="U19:V20"/>
+    <mergeCell ref="AE19:AF20"/>
+    <mergeCell ref="AA19:AB20"/>
+    <mergeCell ref="O21:P22"/>
+    <mergeCell ref="Q21:R22"/>
+    <mergeCell ref="S21:T22"/>
+    <mergeCell ref="U21:V22"/>
+    <mergeCell ref="W21:X22"/>
     <mergeCell ref="K21:L22"/>
     <mergeCell ref="M21:N22"/>
     <mergeCell ref="W19:X20"/>
@@ -3384,23 +3351,38 @@
     <mergeCell ref="AC19:AD20"/>
     <mergeCell ref="AG17:AH18"/>
     <mergeCell ref="AG19:AH20"/>
-    <mergeCell ref="O21:P22"/>
-    <mergeCell ref="Q21:R22"/>
-    <mergeCell ref="S21:T22"/>
-    <mergeCell ref="U21:V22"/>
-    <mergeCell ref="W21:X22"/>
-    <mergeCell ref="O19:P20"/>
-    <mergeCell ref="Q19:R20"/>
-    <mergeCell ref="S19:T20"/>
-    <mergeCell ref="U19:V20"/>
-    <mergeCell ref="AE19:AF20"/>
-    <mergeCell ref="AE21:AF22"/>
-    <mergeCell ref="Y21:Z22"/>
-    <mergeCell ref="AA21:AB22"/>
-    <mergeCell ref="AG21:AH22"/>
-    <mergeCell ref="AI21:AJ22"/>
-    <mergeCell ref="AA19:AB20"/>
-    <mergeCell ref="AI19:AJ20"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="D21:E22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="H17:I18"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="D19:E20"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="N6:O7"/>
+    <mergeCell ref="B15:E16"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="D17:E18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="H6:I7"/>
+    <mergeCell ref="J6:K7"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="O15:AH16"/>
+    <mergeCell ref="Q17:AF18"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="F2:M3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:E5"/>
+    <mergeCell ref="F4:G5"/>
+    <mergeCell ref="H4:M5"/>
+    <mergeCell ref="N4:O5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated protocol excel doc
</commit_message>
<xml_diff>
--- a/DOC/Packet Structure.xlsx
+++ b/DOC/Packet Structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ProiectLicenta\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A14956-B6A9-4AB8-ACE6-35DC82C462ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB287EDB-C53E-44FC-A57B-7B13D26212E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documantation" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="73">
   <si>
     <t>HEAD</t>
   </si>
@@ -144,9 +144,6 @@
     <t>0x00-0xFF</t>
   </si>
   <si>
-    <t>0xAB/0xAC</t>
-  </si>
-  <si>
     <t>Slope Type</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>MILISECS_SH</t>
   </si>
   <si>
-    <t>Aditional info for the optional data bytes                                                                                                                                                0xAB (Time Stamp and Slope)                                                                                                    YEAR Byte will be saved as a single byte by substracting '2000'                              SLOPE (ST - SLOPE TYPE)                                                                                                                  0x01 For rising slope                                                                                                                       0x10 For falling slope                                                                                                                             0xAC (Boot up)                                                                                                                                          No extra data bytes, the type byte means the board booted up                             MILSECS_FH(FIRST HALF) AND MILSECS_SH(SECOND HALF) represents the millisecond that the signal triggerd, to get the milisecond the next steps will be taken: transform the bytes from base 16 to base 10, than               MILSECS_FH(b10) * 100 + MILSECS_SH(b10)</t>
-  </si>
-  <si>
     <t>AA0AAB18041C160B2607030135</t>
   </si>
   <si>
@@ -232,6 +226,36 @@
   </si>
   <si>
     <t>SECOND</t>
+  </si>
+  <si>
+    <t>0xAX</t>
+  </si>
+  <si>
+    <t>0xAD</t>
+  </si>
+  <si>
+    <t>IP B1</t>
+  </si>
+  <si>
+    <t>IP B2</t>
+  </si>
+  <si>
+    <t>IP B3</t>
+  </si>
+  <si>
+    <t>IP B4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETH CONNECTION STATUS </t>
+  </si>
+  <si>
+    <t>IP ADRESS OF THE BOARD</t>
+  </si>
+  <si>
+    <t>ETH CONNECTION BYTE</t>
+  </si>
+  <si>
+    <t>Aditional info for the optional data bytes                                                                                                                                                0xAB (Time Stamp and Slope)                                                                                                    YEAR Byte will be saved as a single byte by substracting '2000'  (to get the year from the packet, the value 2000 should be added)                                                               SLOPE (ST - SLOPE TYPE)                                                                                                                  0x01 For rising slope                                                                                                                       0x10 For falling slope                                                                                            MILSECS_FH(FIRST HALF) AND MILSECS_SH(SECOND HALF) represents the millisecond that the signal triggerd, to get the milisecond the next steps will be taken: transform the bytes from base 16 to base 10, than               MILSECS_FH(b10) * 100 + MILSECS_SH(b10)                                                                                                                              0xAC (Boot up)                                                                                                                                          No extra data bytes, the type byte means the board booted up                                                                                                                     0xAD (ETH CONNECTION STATUS) if ETH CONNECTION BYTE is 0x01 the board is connected to ethernet, oterwise if ETH CONNECTION BYTE is 0x00 the board is not connected and the ip bytes will all be 0x00</t>
   </si>
 </sst>
 </file>
@@ -329,7 +353,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="95">
+  <borders count="101">
     <border>
       <left/>
       <right/>
@@ -1365,13 +1389,75 @@
       <bottom style="thick">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1439,226 +1525,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1670,9 +1537,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1703,6 +1579,219 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1757,56 +1846,80 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="97" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2101,10 +2214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:X46"/>
+  <dimension ref="E5:X48"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2115,32 +2228,32 @@
     <col min="16" max="16" width="13.28515625" style="1" customWidth="1"/>
     <col min="17" max="20" width="12.7109375" style="1" customWidth="1"/>
     <col min="21" max="21" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="5:22" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="53" t="s">
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="55"/>
-      <c r="Q6" s="59" t="s">
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="R6" s="60"/>
+      <c r="R6" s="68"/>
       <c r="T6" s="13" t="s">
         <v>29</v>
       </c>
@@ -2152,149 +2265,149 @@
       </c>
     </row>
     <row r="7" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="84"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="57"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="61"/>
-      <c r="R7" s="62"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="69"/>
+      <c r="R7" s="70"/>
       <c r="T7" s="13" t="s">
         <v>30</v>
       </c>
       <c r="U7" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="V7" s="15" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="5:22" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="75" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="76"/>
-      <c r="G8" s="79" t="s">
+      <c r="E8" s="84" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="85"/>
+      <c r="G8" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="80"/>
-      <c r="I8" s="93" t="s">
+      <c r="H8" s="89"/>
+      <c r="I8" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="94"/>
-      <c r="K8" s="87" t="s">
+      <c r="J8" s="103"/>
+      <c r="K8" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="88"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="89"/>
-      <c r="Q8" s="49" t="s">
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="97"/>
+      <c r="O8" s="97"/>
+      <c r="P8" s="98"/>
+      <c r="Q8" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="R8" s="50"/>
+      <c r="R8" s="58"/>
       <c r="T8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="U8" s="14" t="s">
+      <c r="V8" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="86"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="91"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="100"/>
+      <c r="M9" s="100"/>
+      <c r="N9" s="100"/>
+      <c r="O9" s="100"/>
+      <c r="P9" s="101"/>
+      <c r="Q9" s="59"/>
+      <c r="R9" s="60"/>
+      <c r="T9" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="V8" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="77"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="96"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="91"/>
-      <c r="M9" s="91"/>
-      <c r="N9" s="91"/>
-      <c r="O9" s="91"/>
-      <c r="P9" s="92"/>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="52"/>
-      <c r="T9" s="13" t="s">
-        <v>41</v>
-      </c>
       <c r="U9" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V9" s="15" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="5:22" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="27" t="s">
+      <c r="F10" s="81"/>
+      <c r="G10" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="28"/>
-      <c r="I10" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="L10" s="31"/>
-      <c r="M10" s="28" t="s">
+      <c r="H10" s="80"/>
+      <c r="I10" s="106" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="81"/>
+      <c r="K10" s="106" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="81"/>
+      <c r="M10" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="N10" s="28"/>
-      <c r="O10" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="28" t="s">
+      <c r="N10" s="80"/>
+      <c r="O10" s="106" t="s">
+        <v>40</v>
+      </c>
+      <c r="P10" s="81"/>
+      <c r="Q10" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="R10" s="31"/>
+      <c r="R10" s="81"/>
       <c r="T10" s="13" t="s">
         <v>26</v>
       </c>
       <c r="U10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="V10" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="V10" s="15" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="11" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="29"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="32"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="107"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="107"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="107"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="82"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="83"/>
+      <c r="Q11" s="82"/>
+      <c r="R11" s="83"/>
       <c r="T11" s="13" t="s">
         <v>31</v>
       </c>
       <c r="U11" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V11" s="15" t="s">
         <v>34</v>
@@ -2303,15 +2416,15 @@
     <row r="12" spans="5:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="5:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="63" t="str">
+      <c r="E15" s="27" t="str">
         <f>E6</f>
         <v>HEADER BYTES</v>
       </c>
-      <c r="F15" s="64"/>
+      <c r="F15" s="28"/>
     </row>
     <row r="16" spans="5:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="30"/>
     </row>
     <row r="17" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E17" s="4"/>
@@ -2319,34 +2432,34 @@
     <row r="18" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" s="3"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="67" t="str">
+      <c r="G18" s="72" t="str">
         <f>E8</f>
         <v>START</v>
       </c>
-      <c r="H18" s="68"/>
-      <c r="I18" s="37" t="s">
+      <c r="H18" s="73"/>
+      <c r="I18" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="38"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="39"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="47"/>
     </row>
     <row r="19" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E19" s="2"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="42"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="49"/>
+      <c r="O19" s="49"/>
+      <c r="P19" s="50"/>
     </row>
     <row r="20" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20" s="2"/>
@@ -2354,195 +2467,203 @@
     <row r="21" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E21" s="2"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="71" t="str">
+      <c r="G21" s="76" t="str">
         <f>G8</f>
         <v>DATA SIZE</v>
       </c>
-      <c r="H21" s="72"/>
-      <c r="I21" s="43" t="s">
+      <c r="H21" s="77"/>
+      <c r="I21" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="45"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="53"/>
     </row>
     <row r="22" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G22" s="73"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="47"/>
-      <c r="P22" s="48"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="56"/>
     </row>
     <row r="23" spans="5:24" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S24" s="17"/>
+    </row>
     <row r="25" spans="5:24" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="33" t="str">
+      <c r="E25" s="41" t="str">
         <f>I6</f>
         <v>DATA BYTES</v>
       </c>
-      <c r="F25" s="34"/>
+      <c r="F25" s="42"/>
     </row>
     <row r="26" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="44"/>
     </row>
     <row r="27" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E27" s="3"/>
+      <c r="S27" s="154" t="s">
+        <v>72</v>
+      </c>
+      <c r="T27" s="154"/>
+      <c r="U27" s="154"/>
+      <c r="V27" s="154"/>
+      <c r="W27" s="154"/>
+      <c r="X27" s="154"/>
     </row>
     <row r="28" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E28" s="3"/>
-      <c r="G28" s="122" t="str">
+      <c r="G28" s="123" t="str">
         <f>I8</f>
         <v>PACKET TYPE</v>
       </c>
-      <c r="H28" s="123"/>
-      <c r="I28" s="37" t="s">
+      <c r="H28" s="124"/>
+      <c r="I28" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="126" t="s">
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="N28" s="127"/>
-      <c r="O28" s="127"/>
-      <c r="P28" s="128"/>
+      <c r="N28" s="128"/>
+      <c r="O28" s="128"/>
+      <c r="P28" s="129"/>
       <c r="R28" s="20"/>
-      <c r="S28" s="129" t="s">
-        <v>56</v>
-      </c>
-      <c r="T28" s="129"/>
-      <c r="U28" s="129"/>
-      <c r="V28" s="129"/>
-      <c r="W28" s="129"/>
-      <c r="X28" s="129"/>
+      <c r="S28" s="154"/>
+      <c r="T28" s="154"/>
+      <c r="U28" s="154"/>
+      <c r="V28" s="154"/>
+      <c r="W28" s="154"/>
+      <c r="X28" s="154"/>
     </row>
     <row r="29" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E29" s="2"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="124"/>
-      <c r="H29" s="125"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="126" t="s">
+      <c r="G29" s="125"/>
+      <c r="H29" s="126"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="N29" s="127"/>
-      <c r="O29" s="127"/>
-      <c r="P29" s="128"/>
+      <c r="N29" s="128"/>
+      <c r="O29" s="128"/>
+      <c r="P29" s="129"/>
       <c r="R29" s="20"/>
-      <c r="S29" s="129"/>
-      <c r="T29" s="129"/>
-      <c r="U29" s="129"/>
-      <c r="V29" s="129"/>
-      <c r="W29" s="129"/>
-      <c r="X29" s="129"/>
+      <c r="S29" s="154"/>
+      <c r="T29" s="154"/>
+      <c r="U29" s="154"/>
+      <c r="V29" s="154"/>
+      <c r="W29" s="154"/>
+      <c r="X29" s="154"/>
     </row>
     <row r="30" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E30" s="2"/>
       <c r="R30" s="20"/>
-      <c r="S30" s="129"/>
-      <c r="T30" s="129"/>
-      <c r="U30" s="129"/>
-      <c r="V30" s="129"/>
-      <c r="W30" s="129"/>
-      <c r="X30" s="129"/>
+      <c r="S30" s="154"/>
+      <c r="T30" s="154"/>
+      <c r="U30" s="154"/>
+      <c r="V30" s="154"/>
+      <c r="W30" s="154"/>
+      <c r="X30" s="154"/>
     </row>
     <row r="31" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E31" s="2"/>
-      <c r="G31" s="111" t="s">
+      <c r="G31" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="112"/>
-      <c r="I31" s="116" t="s">
-        <v>53</v>
-      </c>
-      <c r="J31" s="117"/>
-      <c r="K31" s="117"/>
-      <c r="L31" s="117"/>
-      <c r="M31" s="117"/>
-      <c r="N31" s="117"/>
-      <c r="O31" s="117"/>
-      <c r="P31" s="118"/>
+      <c r="H31" s="113"/>
+      <c r="I31" s="117" t="s">
+        <v>52</v>
+      </c>
+      <c r="J31" s="118"/>
+      <c r="K31" s="118"/>
+      <c r="L31" s="118"/>
+      <c r="M31" s="118"/>
+      <c r="N31" s="118"/>
+      <c r="O31" s="118"/>
+      <c r="P31" s="119"/>
       <c r="R31" s="20"/>
-      <c r="S31" s="129"/>
-      <c r="T31" s="129"/>
-      <c r="U31" s="129"/>
-      <c r="V31" s="129"/>
-      <c r="W31" s="129"/>
-      <c r="X31" s="129"/>
+      <c r="S31" s="154"/>
+      <c r="T31" s="154"/>
+      <c r="U31" s="154"/>
+      <c r="V31" s="154"/>
+      <c r="W31" s="154"/>
+      <c r="X31" s="154"/>
     </row>
     <row r="32" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F32" s="8"/>
-      <c r="G32" s="113"/>
-      <c r="H32" s="114"/>
-      <c r="I32" s="119"/>
-      <c r="J32" s="120"/>
-      <c r="K32" s="120"/>
-      <c r="L32" s="120"/>
-      <c r="M32" s="120"/>
-      <c r="N32" s="120"/>
-      <c r="O32" s="120"/>
-      <c r="P32" s="121"/>
+      <c r="G32" s="114"/>
+      <c r="H32" s="115"/>
+      <c r="I32" s="120"/>
+      <c r="J32" s="121"/>
+      <c r="K32" s="121"/>
+      <c r="L32" s="121"/>
+      <c r="M32" s="121"/>
+      <c r="N32" s="121"/>
+      <c r="O32" s="121"/>
+      <c r="P32" s="122"/>
       <c r="R32" s="20"/>
-      <c r="S32" s="129"/>
-      <c r="T32" s="129"/>
-      <c r="U32" s="129"/>
-      <c r="V32" s="129"/>
-      <c r="W32" s="129"/>
-      <c r="X32" s="129"/>
+      <c r="S32" s="154"/>
+      <c r="T32" s="154"/>
+      <c r="U32" s="154"/>
+      <c r="V32" s="154"/>
+      <c r="W32" s="154"/>
+      <c r="X32" s="154"/>
     </row>
     <row r="33" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G33" s="9"/>
       <c r="R33" s="20"/>
-      <c r="S33" s="129"/>
-      <c r="T33" s="129"/>
-      <c r="U33" s="129"/>
-      <c r="V33" s="129"/>
-      <c r="W33" s="129"/>
-      <c r="X33" s="129"/>
+      <c r="S33" s="154"/>
+      <c r="T33" s="154"/>
+      <c r="U33" s="154"/>
+      <c r="V33" s="154"/>
+      <c r="W33" s="154"/>
+      <c r="X33" s="154"/>
     </row>
     <row r="34" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="115" t="s">
+      <c r="G34" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="115"/>
-      <c r="I34" s="23" t="s">
+      <c r="H34" s="116"/>
+      <c r="I34" s="108" t="s">
         <v>23</v>
       </c>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="24"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="26"/>
+      <c r="J34" s="109"/>
+      <c r="K34" s="109"/>
+      <c r="L34" s="109"/>
+      <c r="M34" s="109"/>
+      <c r="N34" s="109"/>
+      <c r="O34" s="110"/>
+      <c r="P34" s="111"/>
       <c r="Q34" s="10" t="s">
         <v>22</v>
       </c>
       <c r="R34" s="20"/>
-      <c r="S34" s="129"/>
-      <c r="T34" s="129"/>
-      <c r="U34" s="129"/>
-      <c r="V34" s="129"/>
-      <c r="W34" s="129"/>
-      <c r="X34" s="129"/>
+      <c r="S34" s="154"/>
+      <c r="T34" s="154"/>
+      <c r="U34" s="154"/>
+      <c r="V34" s="154"/>
+      <c r="W34" s="154"/>
+      <c r="X34" s="154"/>
     </row>
     <row r="35" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G35" s="115"/>
-      <c r="H35" s="115"/>
+      <c r="G35" s="116"/>
+      <c r="H35" s="116"/>
       <c r="I35" s="10" t="s">
         <v>16</v>
       </c>
@@ -2562,155 +2683,247 @@
         <v>21</v>
       </c>
       <c r="O35" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="P35" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="P35" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="Q35" s="22" t="s">
         <v>26</v>
       </c>
       <c r="R35" s="20"/>
-      <c r="S35" s="129"/>
-      <c r="T35" s="129"/>
-      <c r="U35" s="129"/>
-      <c r="V35" s="129"/>
-      <c r="W35" s="129"/>
-      <c r="X35" s="129"/>
+      <c r="S35" s="154"/>
+      <c r="T35" s="154"/>
+      <c r="U35" s="154"/>
+      <c r="V35" s="154"/>
+      <c r="W35" s="154"/>
+      <c r="X35" s="154"/>
     </row>
     <row r="36" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G36" s="11"/>
       <c r="R36" s="20"/>
-      <c r="S36" s="129"/>
-      <c r="T36" s="129"/>
-      <c r="U36" s="129"/>
-      <c r="V36" s="129"/>
-      <c r="W36" s="129"/>
-      <c r="X36" s="129"/>
+      <c r="S36" s="154"/>
+      <c r="T36" s="154"/>
+      <c r="U36" s="154"/>
+      <c r="V36" s="154"/>
+      <c r="W36" s="154"/>
+      <c r="X36" s="154"/>
     </row>
     <row r="37" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="G37" s="98" t="s">
+      <c r="G37" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="98"/>
-      <c r="I37" s="98" t="s">
+      <c r="H37" s="25"/>
+      <c r="I37" s="146" t="s">
         <v>25</v>
       </c>
-      <c r="J37" s="98"/>
-      <c r="K37" s="98"/>
-      <c r="L37" s="98"/>
-      <c r="M37" s="98"/>
-      <c r="N37" s="98"/>
-      <c r="O37" s="98"/>
+      <c r="J37" s="110"/>
+      <c r="K37" s="110"/>
+      <c r="L37" s="110"/>
+      <c r="M37" s="110"/>
+      <c r="N37" s="110"/>
+      <c r="O37" s="110"/>
+      <c r="P37" s="111"/>
       <c r="R37" s="20"/>
-      <c r="S37" s="129"/>
-      <c r="T37" s="129"/>
-      <c r="U37" s="129"/>
-      <c r="V37" s="129"/>
-      <c r="W37" s="129"/>
-      <c r="X37" s="129"/>
+      <c r="S37" s="154"/>
+      <c r="T37" s="154"/>
+      <c r="U37" s="154"/>
+      <c r="V37" s="154"/>
+      <c r="W37" s="154"/>
+      <c r="X37" s="154"/>
     </row>
     <row r="38" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G38" s="99"/>
-      <c r="H38" s="99"/>
-      <c r="I38" s="99"/>
-      <c r="J38" s="99"/>
-      <c r="K38" s="99"/>
-      <c r="L38" s="99"/>
-      <c r="M38" s="99"/>
-      <c r="N38" s="99"/>
-      <c r="O38" s="99"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="147"/>
+      <c r="J38" s="148"/>
+      <c r="K38" s="148"/>
+      <c r="L38" s="148"/>
+      <c r="M38" s="148"/>
+      <c r="N38" s="148"/>
+      <c r="O38" s="148"/>
+      <c r="P38" s="149"/>
       <c r="R38" s="20"/>
-      <c r="S38" s="129"/>
-      <c r="T38" s="129"/>
-      <c r="U38" s="129"/>
-      <c r="V38" s="129"/>
-      <c r="W38" s="129"/>
-      <c r="X38" s="129"/>
-    </row>
-    <row r="40" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="5:24" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E41" s="63" t="str">
+      <c r="S38" s="154"/>
+      <c r="T38" s="154"/>
+      <c r="U38" s="154"/>
+      <c r="V38" s="154"/>
+      <c r="W38" s="154"/>
+      <c r="X38" s="154"/>
+    </row>
+    <row r="39" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G39" s="150"/>
+      <c r="S39" s="154"/>
+      <c r="T39" s="154"/>
+      <c r="U39" s="154"/>
+      <c r="V39" s="154"/>
+      <c r="W39" s="154"/>
+      <c r="X39" s="154"/>
+    </row>
+    <row r="40" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G40" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" s="25"/>
+      <c r="I40" s="108" t="s">
+        <v>70</v>
+      </c>
+      <c r="J40" s="109"/>
+      <c r="K40" s="109"/>
+      <c r="L40" s="151"/>
+      <c r="M40" s="108" t="s">
+        <v>69</v>
+      </c>
+      <c r="N40" s="109"/>
+      <c r="O40" s="151"/>
+      <c r="P40" s="152"/>
+      <c r="S40" s="154"/>
+      <c r="T40" s="154"/>
+      <c r="U40" s="154"/>
+      <c r="V40" s="154"/>
+      <c r="W40" s="154"/>
+      <c r="X40" s="154"/>
+    </row>
+    <row r="41" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="J41" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="K41" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="L41" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="M41" s="147" t="s">
+        <v>71</v>
+      </c>
+      <c r="N41" s="148"/>
+      <c r="O41" s="149"/>
+      <c r="P41" s="153"/>
+      <c r="S41" s="154"/>
+      <c r="T41" s="154"/>
+      <c r="U41" s="154"/>
+      <c r="V41" s="154"/>
+      <c r="W41" s="154"/>
+      <c r="X41" s="154"/>
+    </row>
+    <row r="42" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S42" s="154"/>
+      <c r="T42" s="154"/>
+      <c r="U42" s="154"/>
+      <c r="V42" s="154"/>
+      <c r="W42" s="154"/>
+      <c r="X42" s="154"/>
+    </row>
+    <row r="43" spans="5:24" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="27" t="str">
         <f>Q6</f>
         <v>END BYTE</v>
       </c>
-      <c r="F41" s="64"/>
-    </row>
-    <row r="42" spans="5:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E42" s="100"/>
-      <c r="F42" s="66"/>
-    </row>
-    <row r="43" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E43" s="4"/>
-      <c r="R43" s="97" t="s">
+      <c r="F43" s="28"/>
+      <c r="R43" s="20"/>
+      <c r="S43" s="20"/>
+      <c r="T43" s="20"/>
+      <c r="U43" s="20"/>
+      <c r="V43" s="20"/>
+      <c r="W43" s="20"/>
+    </row>
+    <row r="44" spans="5:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E44" s="29"/>
+      <c r="F44" s="30"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="20"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="20"/>
+      <c r="W44" s="20"/>
+    </row>
+    <row r="45" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E45" s="4"/>
+      <c r="R45" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="S43" s="97"/>
-      <c r="T43" s="97"/>
-      <c r="U43" s="97"/>
-      <c r="V43" s="97"/>
-      <c r="W43" s="97"/>
-    </row>
-    <row r="44" spans="5:24" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E44" s="3"/>
-      <c r="G44" s="101" t="str">
+      <c r="S45" s="24"/>
+      <c r="T45" s="24"/>
+      <c r="U45" s="24"/>
+      <c r="V45" s="24"/>
+      <c r="W45" s="24"/>
+      <c r="X45" s="24"/>
+    </row>
+    <row r="46" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E46" s="3"/>
+      <c r="G46" s="31" t="str">
         <f>Q8</f>
         <v>CHECK SUM</v>
       </c>
-      <c r="H44" s="102"/>
-      <c r="I44" s="105" t="s">
+      <c r="H46" s="32"/>
+      <c r="I46" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="J44" s="106"/>
-      <c r="K44" s="106"/>
-      <c r="L44" s="106"/>
-      <c r="M44" s="106"/>
-      <c r="N44" s="106"/>
-      <c r="O44" s="106"/>
-      <c r="P44" s="107"/>
-      <c r="R44" s="97"/>
-      <c r="S44" s="97"/>
-      <c r="T44" s="97"/>
-      <c r="U44" s="97"/>
-      <c r="V44" s="97"/>
-      <c r="W44" s="97"/>
-    </row>
-    <row r="45" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F45" s="12"/>
-      <c r="G45" s="103"/>
-      <c r="H45" s="104"/>
-      <c r="I45" s="108"/>
-      <c r="J45" s="109"/>
-      <c r="K45" s="109"/>
-      <c r="L45" s="109"/>
-      <c r="M45" s="109"/>
-      <c r="N45" s="109"/>
-      <c r="O45" s="109"/>
-      <c r="P45" s="110"/>
-      <c r="R45" s="97"/>
-      <c r="S45" s="97"/>
-      <c r="T45" s="97"/>
-      <c r="U45" s="97"/>
-      <c r="V45" s="97"/>
-      <c r="W45" s="97"/>
-    </row>
-    <row r="46" spans="5:24" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="R46" s="97"/>
-      <c r="S46" s="97"/>
-      <c r="T46" s="97"/>
-      <c r="U46" s="97"/>
-      <c r="V46" s="97"/>
-      <c r="W46" s="97"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="36"/>
+      <c r="M46" s="36"/>
+      <c r="N46" s="36"/>
+      <c r="O46" s="36"/>
+      <c r="P46" s="37"/>
+      <c r="R46" s="24"/>
+      <c r="S46" s="24"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="24"/>
+      <c r="W46" s="24"/>
+      <c r="X46" s="24"/>
+    </row>
+    <row r="47" spans="5:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F47" s="12"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="39"/>
+      <c r="L47" s="39"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="39"/>
+      <c r="O47" s="39"/>
+      <c r="P47" s="40"/>
+      <c r="R47" s="24"/>
+      <c r="S47" s="24"/>
+      <c r="T47" s="24"/>
+      <c r="U47" s="24"/>
+      <c r="V47" s="24"/>
+      <c r="W47" s="24"/>
+      <c r="X47" s="24"/>
+    </row>
+    <row r="48" spans="5:24" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R48" s="24"/>
+      <c r="S48" s="24"/>
+      <c r="T48" s="24"/>
+      <c r="U48" s="24"/>
+      <c r="V48" s="24"/>
+      <c r="W48" s="24"/>
+      <c r="X48" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="R43:W46"/>
-    <mergeCell ref="G37:H38"/>
-    <mergeCell ref="I37:O38"/>
-    <mergeCell ref="E41:F42"/>
-    <mergeCell ref="G44:H45"/>
-    <mergeCell ref="I44:P45"/>
-    <mergeCell ref="S28:X38"/>
+  <mergeCells count="40">
+    <mergeCell ref="R45:X48"/>
+    <mergeCell ref="S27:X42"/>
+    <mergeCell ref="I46:P47"/>
+    <mergeCell ref="G40:H41"/>
+    <mergeCell ref="I37:P38"/>
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="M40:O40"/>
+    <mergeCell ref="G10:H11"/>
+    <mergeCell ref="I10:J11"/>
+    <mergeCell ref="K10:L11"/>
+    <mergeCell ref="M10:N11"/>
+    <mergeCell ref="O10:P11"/>
     <mergeCell ref="E25:F26"/>
     <mergeCell ref="I18:P19"/>
     <mergeCell ref="I21:P22"/>
@@ -2727,12 +2940,9 @@
     <mergeCell ref="K8:P9"/>
     <mergeCell ref="I8:J9"/>
     <mergeCell ref="E10:F11"/>
+    <mergeCell ref="G37:H38"/>
+    <mergeCell ref="E43:F44"/>
     <mergeCell ref="I34:P34"/>
-    <mergeCell ref="G10:H11"/>
-    <mergeCell ref="I10:J11"/>
-    <mergeCell ref="K10:L11"/>
-    <mergeCell ref="M10:N11"/>
-    <mergeCell ref="O10:P11"/>
     <mergeCell ref="G31:H32"/>
     <mergeCell ref="G34:H35"/>
     <mergeCell ref="I31:P32"/>
@@ -2740,6 +2950,7 @@
     <mergeCell ref="I28:L29"/>
     <mergeCell ref="M28:P28"/>
     <mergeCell ref="M29:P29"/>
+    <mergeCell ref="G46:H47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2750,7 +2961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F8F41-6AB8-4FE5-9A10-D5070C0839ED}">
   <dimension ref="B1:AJ32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="AI19" sqref="AI19:AJ20"/>
     </sheetView>
   </sheetViews>
@@ -2766,534 +2977,534 @@
   <sheetData>
     <row r="1" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:36" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="130" t="s">
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="133" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131"/>
-      <c r="K2" s="131"/>
-      <c r="L2" s="131"/>
-      <c r="M2" s="132"/>
-      <c r="N2" s="59" t="s">
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="145"/>
+      <c r="N2" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="60"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="84"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="62"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="70"/>
     </row>
     <row r="4" spans="2:36" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="79" t="s">
+      <c r="C4" s="85"/>
+      <c r="D4" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="93" t="s">
+      <c r="E4" s="89"/>
+      <c r="F4" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="94"/>
-      <c r="H4" s="87" t="s">
+      <c r="G4" s="103"/>
+      <c r="H4" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="49" t="s">
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="50"/>
+      <c r="O4" s="58"/>
     </row>
     <row r="5" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="77"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="52"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="60"/>
     </row>
     <row r="6" spans="2:36" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="27" t="s">
+      <c r="C6" s="81"/>
+      <c r="D6" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" s="31"/>
-      <c r="J6" s="28" t="s">
+      <c r="E6" s="80"/>
+      <c r="F6" s="106" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="81"/>
+      <c r="H6" s="106" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="81"/>
+      <c r="J6" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="28"/>
-      <c r="L6" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="31"/>
-      <c r="N6" s="28" t="s">
+      <c r="K6" s="80"/>
+      <c r="L6" s="106" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="81"/>
+      <c r="N6" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="31"/>
+      <c r="O6" s="81"/>
     </row>
     <row r="7" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="29"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="32"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="83"/>
     </row>
     <row r="8" spans="2:36" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:36" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="130" t="s">
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="133" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="131"/>
-      <c r="H15" s="59" t="s">
+      <c r="G15" s="134"/>
+      <c r="H15" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="60"/>
+      <c r="I15" s="68"/>
       <c r="J15" s="16"/>
-      <c r="K15" s="59" t="s">
+      <c r="K15" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="L15" s="83"/>
-      <c r="M15" s="83"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="53" t="s">
+      <c r="L15" s="92"/>
+      <c r="M15" s="92"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="54"/>
-      <c r="V15" s="54"/>
-      <c r="W15" s="54"/>
-      <c r="X15" s="54"/>
-      <c r="Y15" s="54"/>
-      <c r="Z15" s="54"/>
-      <c r="AA15" s="54"/>
-      <c r="AB15" s="54"/>
-      <c r="AC15" s="54"/>
-      <c r="AD15" s="54"/>
-      <c r="AE15" s="54"/>
-      <c r="AF15" s="54"/>
-      <c r="AG15" s="54"/>
-      <c r="AH15" s="55"/>
-      <c r="AI15" s="59" t="s">
+      <c r="P15" s="62"/>
+      <c r="Q15" s="62"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="62"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="62"/>
+      <c r="V15" s="62"/>
+      <c r="W15" s="62"/>
+      <c r="X15" s="62"/>
+      <c r="Y15" s="62"/>
+      <c r="Z15" s="62"/>
+      <c r="AA15" s="62"/>
+      <c r="AB15" s="62"/>
+      <c r="AC15" s="62"/>
+      <c r="AD15" s="62"/>
+      <c r="AE15" s="62"/>
+      <c r="AF15" s="62"/>
+      <c r="AG15" s="62"/>
+      <c r="AH15" s="63"/>
+      <c r="AI15" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="AJ15" s="60"/>
+      <c r="AJ15" s="68"/>
     </row>
     <row r="16" spans="2:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="84"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="139"/>
-      <c r="G16" s="140"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="62"/>
+      <c r="B16" s="93"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="135"/>
+      <c r="G16" s="136"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="70"/>
       <c r="J16" s="16"/>
-      <c r="K16" s="84"/>
-      <c r="L16" s="85"/>
-      <c r="M16" s="85"/>
-      <c r="N16" s="86"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
-      <c r="R16" s="57"/>
-      <c r="S16" s="57"/>
-      <c r="T16" s="57"/>
-      <c r="U16" s="57"/>
-      <c r="V16" s="57"/>
-      <c r="W16" s="57"/>
-      <c r="X16" s="57"/>
-      <c r="Y16" s="57"/>
-      <c r="Z16" s="57"/>
-      <c r="AA16" s="57"/>
-      <c r="AB16" s="57"/>
-      <c r="AC16" s="57"/>
-      <c r="AD16" s="57"/>
-      <c r="AE16" s="57"/>
-      <c r="AF16" s="57"/>
-      <c r="AG16" s="57"/>
-      <c r="AH16" s="58"/>
-      <c r="AI16" s="61"/>
-      <c r="AJ16" s="62"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="94"/>
+      <c r="M16" s="94"/>
+      <c r="N16" s="95"/>
+      <c r="O16" s="64"/>
+      <c r="P16" s="65"/>
+      <c r="Q16" s="65"/>
+      <c r="R16" s="65"/>
+      <c r="S16" s="65"/>
+      <c r="T16" s="65"/>
+      <c r="U16" s="65"/>
+      <c r="V16" s="65"/>
+      <c r="W16" s="65"/>
+      <c r="X16" s="65"/>
+      <c r="Y16" s="65"/>
+      <c r="Z16" s="65"/>
+      <c r="AA16" s="65"/>
+      <c r="AB16" s="65"/>
+      <c r="AC16" s="65"/>
+      <c r="AD16" s="65"/>
+      <c r="AE16" s="65"/>
+      <c r="AF16" s="65"/>
+      <c r="AG16" s="65"/>
+      <c r="AH16" s="66"/>
+      <c r="AI16" s="69"/>
+      <c r="AJ16" s="70"/>
     </row>
     <row r="17" spans="2:36" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="79" t="s">
+      <c r="C17" s="85"/>
+      <c r="D17" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="80"/>
-      <c r="F17" s="93" t="s">
+      <c r="E17" s="89"/>
+      <c r="F17" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="94"/>
-      <c r="H17" s="141" t="s">
+      <c r="G17" s="103"/>
+      <c r="H17" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="142"/>
+      <c r="I17" s="138"/>
       <c r="J17" s="16"/>
-      <c r="K17" s="75" t="s">
+      <c r="K17" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="L17" s="76"/>
-      <c r="M17" s="79" t="s">
+      <c r="L17" s="85"/>
+      <c r="M17" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="N17" s="80"/>
-      <c r="O17" s="93" t="s">
+      <c r="N17" s="89"/>
+      <c r="O17" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="P17" s="94"/>
-      <c r="Q17" s="87" t="s">
+      <c r="P17" s="103"/>
+      <c r="Q17" s="96" t="s">
+        <v>46</v>
+      </c>
+      <c r="R17" s="97"/>
+      <c r="S17" s="97"/>
+      <c r="T17" s="97"/>
+      <c r="U17" s="97"/>
+      <c r="V17" s="97"/>
+      <c r="W17" s="97"/>
+      <c r="X17" s="97"/>
+      <c r="Y17" s="97"/>
+      <c r="Z17" s="97"/>
+      <c r="AA17" s="97"/>
+      <c r="AB17" s="97"/>
+      <c r="AC17" s="97"/>
+      <c r="AD17" s="97"/>
+      <c r="AE17" s="97"/>
+      <c r="AF17" s="141"/>
+      <c r="AG17" s="96" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH17" s="98"/>
+      <c r="AI17" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ17" s="58"/>
+    </row>
+    <row r="18" spans="2:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="86"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="139"/>
+      <c r="I18" s="140"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="87"/>
+      <c r="M18" s="90"/>
+      <c r="N18" s="91"/>
+      <c r="O18" s="104"/>
+      <c r="P18" s="105"/>
+      <c r="Q18" s="142"/>
+      <c r="R18" s="143"/>
+      <c r="S18" s="143"/>
+      <c r="T18" s="143"/>
+      <c r="U18" s="143"/>
+      <c r="V18" s="143"/>
+      <c r="W18" s="143"/>
+      <c r="X18" s="143"/>
+      <c r="Y18" s="143"/>
+      <c r="Z18" s="143"/>
+      <c r="AA18" s="143"/>
+      <c r="AB18" s="143"/>
+      <c r="AC18" s="143"/>
+      <c r="AD18" s="143"/>
+      <c r="AE18" s="143"/>
+      <c r="AF18" s="144"/>
+      <c r="AG18" s="99"/>
+      <c r="AH18" s="101"/>
+      <c r="AI18" s="59"/>
+      <c r="AJ18" s="60"/>
+    </row>
+    <row r="19" spans="2:36" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="106" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="81"/>
+      <c r="D19" s="106" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="80"/>
+      <c r="F19" s="106" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="81"/>
+      <c r="H19" s="106" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="81"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="106" t="s">
+        <v>29</v>
+      </c>
+      <c r="L19" s="81"/>
+      <c r="M19" s="106" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" s="80"/>
+      <c r="O19" s="106" t="s">
+        <v>38</v>
+      </c>
+      <c r="P19" s="81"/>
+      <c r="Q19" s="106" t="s">
+        <v>16</v>
+      </c>
+      <c r="R19" s="81"/>
+      <c r="S19" s="80" t="s">
+        <v>17</v>
+      </c>
+      <c r="T19" s="80"/>
+      <c r="U19" s="106" t="s">
+        <v>18</v>
+      </c>
+      <c r="V19" s="81"/>
+      <c r="W19" s="106" t="s">
+        <v>60</v>
+      </c>
+      <c r="X19" s="81"/>
+      <c r="Y19" s="80" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z19" s="80"/>
+      <c r="AA19" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB19" s="81"/>
+      <c r="AC19" s="130" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD19" s="130"/>
+      <c r="AE19" s="130" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF19" s="130"/>
+      <c r="AG19" s="106" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH19" s="81"/>
+      <c r="AI19" s="80" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ19" s="81"/>
+    </row>
+    <row r="20" spans="2:36" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="107"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="107"/>
+      <c r="I20" s="83"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="107"/>
+      <c r="L20" s="83"/>
+      <c r="M20" s="107"/>
+      <c r="N20" s="82"/>
+      <c r="O20" s="107"/>
+      <c r="P20" s="83"/>
+      <c r="Q20" s="107"/>
+      <c r="R20" s="83"/>
+      <c r="S20" s="82"/>
+      <c r="T20" s="82"/>
+      <c r="U20" s="107"/>
+      <c r="V20" s="83"/>
+      <c r="W20" s="107"/>
+      <c r="X20" s="83"/>
+      <c r="Y20" s="82"/>
+      <c r="Z20" s="82"/>
+      <c r="AA20" s="107"/>
+      <c r="AB20" s="83"/>
+      <c r="AC20" s="130"/>
+      <c r="AD20" s="130"/>
+      <c r="AE20" s="130"/>
+      <c r="AF20" s="130"/>
+      <c r="AG20" s="107"/>
+      <c r="AH20" s="83"/>
+      <c r="AI20" s="82"/>
+      <c r="AJ20" s="83"/>
+    </row>
+    <row r="21" spans="2:36" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="106" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="81"/>
+      <c r="D21" s="131" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="131"/>
+      <c r="F21" s="131" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="131"/>
+      <c r="H21" s="131" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="131"/>
+      <c r="K21" s="131" t="s">
+        <v>32</v>
+      </c>
+      <c r="L21" s="131"/>
+      <c r="M21" s="131" t="s">
+        <v>56</v>
+      </c>
+      <c r="N21" s="131"/>
+      <c r="O21" s="131" t="s">
+        <v>15</v>
+      </c>
+      <c r="P21" s="131"/>
+      <c r="Q21" s="131" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="88"/>
-      <c r="S17" s="88"/>
-      <c r="T17" s="88"/>
-      <c r="U17" s="88"/>
-      <c r="V17" s="88"/>
-      <c r="W17" s="88"/>
-      <c r="X17" s="88"/>
-      <c r="Y17" s="88"/>
-      <c r="Z17" s="88"/>
-      <c r="AA17" s="88"/>
-      <c r="AB17" s="88"/>
-      <c r="AC17" s="88"/>
-      <c r="AD17" s="88"/>
-      <c r="AE17" s="88"/>
-      <c r="AF17" s="133"/>
-      <c r="AG17" s="87" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH17" s="89"/>
-      <c r="AI17" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ17" s="50"/>
-    </row>
-    <row r="18" spans="2:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="77"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="95"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="143"/>
-      <c r="I18" s="144"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="77"/>
-      <c r="L18" s="78"/>
-      <c r="M18" s="81"/>
-      <c r="N18" s="82"/>
-      <c r="O18" s="95"/>
-      <c r="P18" s="96"/>
-      <c r="Q18" s="134"/>
-      <c r="R18" s="135"/>
-      <c r="S18" s="135"/>
-      <c r="T18" s="135"/>
-      <c r="U18" s="135"/>
-      <c r="V18" s="135"/>
-      <c r="W18" s="135"/>
-      <c r="X18" s="135"/>
-      <c r="Y18" s="135"/>
-      <c r="Z18" s="135"/>
-      <c r="AA18" s="135"/>
-      <c r="AB18" s="135"/>
-      <c r="AC18" s="135"/>
-      <c r="AD18" s="135"/>
-      <c r="AE18" s="135"/>
-      <c r="AF18" s="136"/>
-      <c r="AG18" s="90"/>
-      <c r="AH18" s="92"/>
-      <c r="AI18" s="51"/>
-      <c r="AJ18" s="52"/>
-    </row>
-    <row r="19" spans="2:36" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" s="31"/>
-      <c r="M19" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="N19" s="28"/>
-      <c r="O19" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="R19" s="31"/>
-      <c r="S19" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="T19" s="28"/>
-      <c r="U19" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="V19" s="31"/>
-      <c r="W19" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="X19" s="31"/>
-      <c r="Y19" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z19" s="28"/>
-      <c r="AA19" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB19" s="31"/>
-      <c r="AC19" s="145" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD19" s="145"/>
-      <c r="AE19" s="145" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF19" s="145"/>
-      <c r="AG19" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH19" s="31"/>
-      <c r="AI19" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ19" s="31"/>
-    </row>
-    <row r="20" spans="2:36" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="29"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
-      <c r="U20" s="29"/>
-      <c r="V20" s="32"/>
-      <c r="W20" s="29"/>
-      <c r="X20" s="32"/>
-      <c r="Y20" s="30"/>
-      <c r="Z20" s="30"/>
-      <c r="AA20" s="29"/>
-      <c r="AB20" s="32"/>
-      <c r="AC20" s="145"/>
-      <c r="AD20" s="145"/>
-      <c r="AE20" s="145"/>
-      <c r="AF20" s="145"/>
-      <c r="AG20" s="29"/>
-      <c r="AH20" s="32"/>
-      <c r="AI20" s="30"/>
-      <c r="AJ20" s="32"/>
-    </row>
-    <row r="21" spans="2:36" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="137" t="s">
+      <c r="R21" s="131"/>
+      <c r="S21" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="T21" s="131"/>
+      <c r="U21" s="131" t="s">
+        <v>49</v>
+      </c>
+      <c r="V21" s="131"/>
+      <c r="W21" s="131" t="s">
+        <v>57</v>
+      </c>
+      <c r="X21" s="131"/>
+      <c r="Y21" s="131" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z21" s="131"/>
+      <c r="AA21" s="131" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB21" s="131"/>
+      <c r="AC21" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="137"/>
-      <c r="F21" s="137" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="137"/>
-      <c r="H21" s="137" t="s">
-        <v>46</v>
-      </c>
-      <c r="I21" s="137"/>
-      <c r="K21" s="137" t="s">
-        <v>32</v>
-      </c>
-      <c r="L21" s="137"/>
-      <c r="M21" s="137" t="s">
-        <v>58</v>
-      </c>
-      <c r="N21" s="137"/>
-      <c r="O21" s="137" t="s">
-        <v>15</v>
-      </c>
-      <c r="P21" s="137"/>
-      <c r="Q21" s="137" t="s">
-        <v>48</v>
-      </c>
-      <c r="R21" s="137"/>
-      <c r="S21" s="137" t="s">
-        <v>49</v>
-      </c>
-      <c r="T21" s="137"/>
-      <c r="U21" s="137" t="s">
-        <v>50</v>
-      </c>
-      <c r="V21" s="137"/>
-      <c r="W21" s="137" t="s">
+      <c r="AD21" s="130"/>
+      <c r="AE21" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="X21" s="137"/>
-      <c r="Y21" s="137" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z21" s="137"/>
-      <c r="AA21" s="137" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB21" s="137"/>
-      <c r="AC21" s="145" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD21" s="145"/>
-      <c r="AE21" s="145" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF21" s="145"/>
-      <c r="AG21" s="137" t="s">
+      <c r="AF21" s="130"/>
+      <c r="AG21" s="131" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH21" s="131"/>
+      <c r="AI21" s="131" t="s">
         <v>45</v>
       </c>
-      <c r="AH21" s="137"/>
-      <c r="AI21" s="137" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ21" s="137"/>
+      <c r="AJ21" s="131"/>
     </row>
     <row r="22" spans="2:36" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="29"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="138"/>
-      <c r="E22" s="138"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="138"/>
-      <c r="H22" s="138"/>
-      <c r="I22" s="138"/>
-      <c r="K22" s="138"/>
-      <c r="L22" s="138"/>
-      <c r="M22" s="138"/>
-      <c r="N22" s="138"/>
-      <c r="O22" s="138"/>
-      <c r="P22" s="138"/>
-      <c r="Q22" s="138"/>
-      <c r="R22" s="138"/>
-      <c r="S22" s="138"/>
-      <c r="T22" s="138"/>
-      <c r="U22" s="138"/>
-      <c r="V22" s="138"/>
-      <c r="W22" s="138"/>
-      <c r="X22" s="138"/>
-      <c r="Y22" s="138"/>
-      <c r="Z22" s="138"/>
-      <c r="AA22" s="138"/>
-      <c r="AB22" s="138"/>
-      <c r="AC22" s="145"/>
-      <c r="AD22" s="145"/>
-      <c r="AE22" s="145"/>
-      <c r="AF22" s="145"/>
-      <c r="AG22" s="138"/>
-      <c r="AH22" s="138"/>
-      <c r="AI22" s="138"/>
-      <c r="AJ22" s="138"/>
+      <c r="B22" s="107"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="132"/>
+      <c r="E22" s="132"/>
+      <c r="F22" s="132"/>
+      <c r="G22" s="132"/>
+      <c r="H22" s="132"/>
+      <c r="I22" s="132"/>
+      <c r="K22" s="132"/>
+      <c r="L22" s="132"/>
+      <c r="M22" s="132"/>
+      <c r="N22" s="132"/>
+      <c r="O22" s="132"/>
+      <c r="P22" s="132"/>
+      <c r="Q22" s="132"/>
+      <c r="R22" s="132"/>
+      <c r="S22" s="132"/>
+      <c r="T22" s="132"/>
+      <c r="U22" s="132"/>
+      <c r="V22" s="132"/>
+      <c r="W22" s="132"/>
+      <c r="X22" s="132"/>
+      <c r="Y22" s="132"/>
+      <c r="Z22" s="132"/>
+      <c r="AA22" s="132"/>
+      <c r="AB22" s="132"/>
+      <c r="AC22" s="130"/>
+      <c r="AD22" s="130"/>
+      <c r="AE22" s="130"/>
+      <c r="AF22" s="130"/>
+      <c r="AG22" s="132"/>
+      <c r="AH22" s="132"/>
+      <c r="AI22" s="132"/>
+      <c r="AJ22" s="132"/>
     </row>
     <row r="23" spans="2:36" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:36" x14ac:dyDescent="0.25">
@@ -3318,23 +3529,38 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="AI19:AJ20"/>
-    <mergeCell ref="AE21:AF22"/>
-    <mergeCell ref="Y21:Z22"/>
-    <mergeCell ref="AA21:AB22"/>
-    <mergeCell ref="AG21:AH22"/>
-    <mergeCell ref="AI21:AJ22"/>
-    <mergeCell ref="O19:P20"/>
-    <mergeCell ref="Q19:R20"/>
-    <mergeCell ref="S19:T20"/>
-    <mergeCell ref="U19:V20"/>
-    <mergeCell ref="AE19:AF20"/>
-    <mergeCell ref="AA19:AB20"/>
-    <mergeCell ref="O21:P22"/>
-    <mergeCell ref="Q21:R22"/>
-    <mergeCell ref="S21:T22"/>
-    <mergeCell ref="U21:V22"/>
-    <mergeCell ref="W21:X22"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="F2:M3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:E5"/>
+    <mergeCell ref="F4:G5"/>
+    <mergeCell ref="H4:M5"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="N6:O7"/>
+    <mergeCell ref="B15:E16"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="D17:E18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="H6:I7"/>
+    <mergeCell ref="J6:K7"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="O15:AH16"/>
+    <mergeCell ref="Q17:AF18"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="D21:E22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="H17:I18"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="D19:E20"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="H19:I20"/>
     <mergeCell ref="K21:L22"/>
     <mergeCell ref="M21:N22"/>
     <mergeCell ref="W19:X20"/>
@@ -3351,38 +3577,23 @@
     <mergeCell ref="AC19:AD20"/>
     <mergeCell ref="AG17:AH18"/>
     <mergeCell ref="AG19:AH20"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="D21:E22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="H15:I16"/>
-    <mergeCell ref="H17:I18"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="D19:E20"/>
-    <mergeCell ref="F19:G20"/>
-    <mergeCell ref="H19:I20"/>
-    <mergeCell ref="N6:O7"/>
-    <mergeCell ref="B15:E16"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="D17:E18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="H6:I7"/>
-    <mergeCell ref="J6:K7"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="O15:AH16"/>
-    <mergeCell ref="Q17:AF18"/>
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="F2:M3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:E5"/>
-    <mergeCell ref="F4:G5"/>
-    <mergeCell ref="H4:M5"/>
-    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="O21:P22"/>
+    <mergeCell ref="Q21:R22"/>
+    <mergeCell ref="S21:T22"/>
+    <mergeCell ref="U21:V22"/>
+    <mergeCell ref="W21:X22"/>
+    <mergeCell ref="O19:P20"/>
+    <mergeCell ref="Q19:R20"/>
+    <mergeCell ref="S19:T20"/>
+    <mergeCell ref="U19:V20"/>
+    <mergeCell ref="AE19:AF20"/>
+    <mergeCell ref="AA19:AB20"/>
+    <mergeCell ref="AI19:AJ20"/>
+    <mergeCell ref="AE21:AF22"/>
+    <mergeCell ref="Y21:Z22"/>
+    <mergeCell ref="AA21:AB22"/>
+    <mergeCell ref="AG21:AH22"/>
+    <mergeCell ref="AI21:AJ22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>